<commit_message>
Added json writer, fixed logging
</commit_message>
<xml_diff>
--- a/SCoCS/laba1/laba1/output.xlsx
+++ b/SCoCS/laba1/laba1/output.xlsx
@@ -12,33 +12,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Petrov</t>
-  </si>
-  <si>
-    <t>Petr</t>
-  </si>
-  <si>
-    <t>Petrovich</t>
-  </si>
-  <si>
-    <t>Ivanov</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Ivanovich</t>
-  </si>
-  <si>
-    <t>Sidorov</t>
-  </si>
-  <si>
-    <t>Sidor</t>
-  </si>
-  <si>
-    <t>Sidorovich</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Biguscus</t>
+  </si>
+  <si>
+    <t>Dues</t>
+  </si>
+  <si>
+    <t>Dadalus</t>
+  </si>
+  <si>
+    <t>Anbitus</t>
+  </si>
+  <si>
+    <t>Fatin</t>
+  </si>
+  <si>
+    <t>Fabucus</t>
+  </si>
+  <si>
+    <t>Banulius</t>
+  </si>
+  <si>
+    <t>Dalus</t>
+  </si>
+  <si>
+    <t>Aldator</t>
+  </si>
+  <si>
+    <t>Dibelius</t>
+  </si>
+  <si>
+    <t>Eutin</t>
+  </si>
+  <si>
+    <t>Dadatus</t>
+  </si>
+  <si>
+    <t>Dofritus</t>
+  </si>
+  <si>
+    <t>Bres</t>
+  </si>
+  <si>
+    <t>Dibocus</t>
+  </si>
+  <si>
+    <t>Bedacio</t>
+  </si>
+  <si>
+    <t>Faes</t>
+  </si>
+  <si>
+    <t>Abicus</t>
+  </si>
+  <si>
+    <t>Alfritus</t>
+  </si>
+  <si>
+    <t>Alius</t>
+  </si>
+  <si>
+    <t>Dabecus</t>
+  </si>
+  <si>
+    <t>Bebelus</t>
+  </si>
+  <si>
+    <t>Datus</t>
+  </si>
+  <si>
+    <t>Dibotin</t>
   </si>
   <si>
     <t>Mathematics</t>
@@ -47,10 +92,22 @@
     <t>Physics</t>
   </si>
   <si>
+    <t>History</t>
+  </si>
+  <si>
     <t>Chemistry</t>
   </si>
   <si>
-    <t>Algorithmization</t>
+    <t>Russian Language</t>
+  </si>
+  <si>
+    <t>Foreign Languages</t>
+  </si>
+  <si>
+    <t>Drawing</t>
+  </si>
+  <si>
+    <t>Work</t>
   </si>
   <si>
     <t>Average group rating</t>
@@ -99,7 +156,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -116,7 +173,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="0">
-        <v>6.5</v>
+        <v>5.625</v>
       </c>
     </row>
     <row r="2">
@@ -130,7 +187,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="0">
-        <v>7.25</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="3">
@@ -144,47 +201,149 @@
         <v>8</v>
       </c>
       <c r="D3" s="0">
-        <v>5.75</v>
+        <v>6.625</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0">
-        <v>6.333333333333333</v>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0">
+        <v>5.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0">
-        <v>5.666666666666667</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0">
+        <v>6.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0">
+        <v>4.375</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="0">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0">
+        <v>4.375</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="0">
-        <v>6.5</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="0">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="0">
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="0">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="0">
+        <v>6.625</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="0">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="0">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="0">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="0">
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0">
+        <v>5.5625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>